<commit_message>
add docs pdf snooze office layout
add docs pdf snooze floor plan realtime trace VNC sessions
</commit_message>
<xml_diff>
--- a/docs/Log Pronto Licenses Used (per hour) xls.xlsx
+++ b/docs/Log Pronto Licenses Used (per hour) xls.xlsx
@@ -161,6 +161,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -1234,11 +1235,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="102284672"/>
-        <c:axId val="102286464"/>
+        <c:axId val="98979200"/>
+        <c:axId val="98980992"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="102284672"/>
+        <c:axId val="98979200"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -1255,7 +1256,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="102286464"/>
+        <c:crossAx val="98980992"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1263,7 +1264,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="102286464"/>
+        <c:axId val="98980992"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="266"/>
@@ -1282,7 +1283,7 @@
             <a:prstDash val="sysDot"/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="102284672"/>
+        <c:crossAx val="98979200"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1645,10 +1646,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G410"/>
+  <dimension ref="A1:G460"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A373" workbookViewId="0">
-      <selection activeCell="A379" sqref="A379"/>
+    <sheetView tabSelected="1" topLeftCell="A416" workbookViewId="0">
+      <selection activeCell="A420" sqref="A420"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5822,6 +5823,9 @@
       </c>
     </row>
     <row r="379" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A379">
+        <v>241</v>
+      </c>
       <c r="B379" s="5">
         <v>41849</v>
       </c>
@@ -5830,142 +5834,668 @@
       </c>
     </row>
     <row r="380" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A380">
+        <v>220</v>
+      </c>
       <c r="B380" s="5">
         <v>41849</v>
       </c>
+      <c r="C380" s="4">
+        <v>0.70833333333332904</v>
+      </c>
     </row>
     <row r="381" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A381">
+        <v>140</v>
+      </c>
       <c r="B381" s="5">
         <v>41849</v>
       </c>
+      <c r="C381" s="4">
+        <v>0.72916666666666197</v>
+      </c>
     </row>
     <row r="382" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A382">
+        <v>69</v>
+      </c>
       <c r="B382" s="5">
         <v>41849</v>
       </c>
+      <c r="C382" s="4">
+        <v>0.749999999999995</v>
+      </c>
     </row>
     <row r="383" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A383">
+        <v>53</v>
+      </c>
       <c r="B383" s="5">
         <v>41849</v>
       </c>
+      <c r="C383" s="4">
+        <v>0.77083333333332804</v>
+      </c>
     </row>
     <row r="384" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A384">
+        <v>1</v>
+      </c>
       <c r="B384" s="5">
-        <v>41849</v>
-      </c>
-    </row>
-    <row r="385" spans="2:2" x14ac:dyDescent="0.25">
+        <v>41850</v>
+      </c>
+      <c r="C384" s="4">
+        <v>0.29166666666666669</v>
+      </c>
+    </row>
+    <row r="385" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A385">
+        <v>4</v>
+      </c>
       <c r="B385" s="5">
-        <v>41849</v>
-      </c>
-    </row>
-    <row r="386" spans="2:2" x14ac:dyDescent="0.25">
+        <v>41850</v>
+      </c>
+      <c r="C385" s="4">
+        <v>0.3125</v>
+      </c>
+    </row>
+    <row r="386" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A386">
+        <v>11</v>
+      </c>
       <c r="B386" s="5">
-        <v>41849</v>
-      </c>
-    </row>
-    <row r="387" spans="2:2" x14ac:dyDescent="0.25">
+        <v>41850</v>
+      </c>
+      <c r="C386" s="4">
+        <v>0.33333333333333298</v>
+      </c>
+    </row>
+    <row r="387" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A387">
+        <v>30</v>
+      </c>
       <c r="B387" s="5">
-        <v>41849</v>
-      </c>
-    </row>
-    <row r="388" spans="2:2" x14ac:dyDescent="0.25">
+        <v>41850</v>
+      </c>
+      <c r="C387" s="4">
+        <v>0.35416666666666702</v>
+      </c>
+    </row>
+    <row r="388" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A388">
+        <v>82</v>
+      </c>
       <c r="B388" s="5">
-        <v>41849</v>
-      </c>
-    </row>
-    <row r="389" spans="2:2" x14ac:dyDescent="0.25">
+        <v>41850</v>
+      </c>
+      <c r="C388" s="4">
+        <v>0.375</v>
+      </c>
+    </row>
+    <row r="389" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A389">
+        <v>170</v>
+      </c>
       <c r="B389" s="5">
-        <v>41849</v>
-      </c>
-    </row>
-    <row r="390" spans="2:2" x14ac:dyDescent="0.25">
+        <v>41850</v>
+      </c>
+      <c r="C389" s="4">
+        <v>0.39583333333333398</v>
+      </c>
+    </row>
+    <row r="390" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A390">
+        <v>203</v>
+      </c>
       <c r="B390" s="5">
-        <v>41849</v>
-      </c>
-    </row>
-    <row r="391" spans="2:2" x14ac:dyDescent="0.25">
+        <v>41850</v>
+      </c>
+      <c r="C390" s="4">
+        <v>0.41666666666666702</v>
+      </c>
+    </row>
+    <row r="391" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A391">
+        <v>217</v>
+      </c>
       <c r="B391" s="5">
-        <v>41849</v>
-      </c>
-    </row>
-    <row r="392" spans="2:2" x14ac:dyDescent="0.25">
+        <v>41850</v>
+      </c>
+      <c r="C391" s="4">
+        <v>0.4375</v>
+      </c>
+    </row>
+    <row r="392" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A392">
+        <v>224</v>
+      </c>
       <c r="B392" s="5">
-        <v>41849</v>
-      </c>
-    </row>
-    <row r="393" spans="2:2" x14ac:dyDescent="0.25">
+        <v>41850</v>
+      </c>
+      <c r="C392" s="4">
+        <v>0.45833333333333398</v>
+      </c>
+    </row>
+    <row r="393" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A393">
+        <v>238</v>
+      </c>
       <c r="B393" s="5">
-        <v>41849</v>
-      </c>
-    </row>
-    <row r="394" spans="2:2" x14ac:dyDescent="0.25">
+        <v>41850</v>
+      </c>
+      <c r="C393" s="4">
+        <v>0.47916666666666802</v>
+      </c>
+    </row>
+    <row r="394" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A394">
+        <v>244</v>
+      </c>
       <c r="B394" s="5">
-        <v>41849</v>
-      </c>
-    </row>
-    <row r="395" spans="2:2" x14ac:dyDescent="0.25">
+        <v>41850</v>
+      </c>
+      <c r="C394" s="4">
+        <v>0.500000000000002</v>
+      </c>
+    </row>
+    <row r="395" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A395">
+        <v>244</v>
+      </c>
       <c r="B395" s="5">
-        <v>41849</v>
-      </c>
-    </row>
-    <row r="396" spans="2:2" x14ac:dyDescent="0.25">
+        <v>41850</v>
+      </c>
+      <c r="C395" s="4">
+        <v>0.52083333333333603</v>
+      </c>
+    </row>
+    <row r="396" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A396">
+        <v>247</v>
+      </c>
       <c r="B396" s="5">
-        <v>41849</v>
-      </c>
-    </row>
-    <row r="397" spans="2:2" x14ac:dyDescent="0.25">
+        <v>41850</v>
+      </c>
+      <c r="C396" s="4">
+        <v>0.54166666666666996</v>
+      </c>
+    </row>
+    <row r="397" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A397">
+        <v>251</v>
+      </c>
       <c r="B397" s="5">
-        <v>41849</v>
-      </c>
-    </row>
-    <row r="398" spans="2:2" x14ac:dyDescent="0.25">
+        <v>41850</v>
+      </c>
+      <c r="C397" s="4">
+        <v>0.562500000000004</v>
+      </c>
+    </row>
+    <row r="398" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A398">
+        <v>250</v>
+      </c>
       <c r="B398" s="5">
-        <v>41849</v>
-      </c>
-    </row>
-    <row r="399" spans="2:2" x14ac:dyDescent="0.25">
+        <v>41850</v>
+      </c>
+      <c r="C398" s="4">
+        <v>0.58333333333333803</v>
+      </c>
+    </row>
+    <row r="399" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A399">
+        <v>250</v>
+      </c>
       <c r="B399" s="5">
-        <v>41849</v>
-      </c>
-    </row>
-    <row r="402" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A402" t="s">
+        <v>41850</v>
+      </c>
+      <c r="C399" s="4">
+        <v>0.60416666666667196</v>
+      </c>
+    </row>
+    <row r="400" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A400">
+        <v>257</v>
+      </c>
+      <c r="B400" s="5">
+        <v>41850</v>
+      </c>
+      <c r="C400" s="4">
+        <v>0.625000000000006</v>
+      </c>
+    </row>
+    <row r="401" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A401">
+        <v>254</v>
+      </c>
+      <c r="B401" s="5">
+        <v>41850</v>
+      </c>
+      <c r="C401" s="4">
+        <v>0.64583333333334003</v>
+      </c>
+    </row>
+    <row r="402" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A402">
+        <v>245</v>
+      </c>
+      <c r="B402" s="5">
+        <v>41850</v>
+      </c>
+      <c r="C402" s="4">
+        <v>0.66666666666667396</v>
+      </c>
+    </row>
+    <row r="403" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A403">
+        <v>231</v>
+      </c>
+      <c r="B403" s="5">
+        <v>41850</v>
+      </c>
+      <c r="C403" s="4">
+        <v>0.68750000000000799</v>
+      </c>
+    </row>
+    <row r="404" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A404">
+        <v>205</v>
+      </c>
+      <c r="B404" s="5">
+        <v>41850</v>
+      </c>
+      <c r="C404" s="4">
+        <v>0.70833333333334203</v>
+      </c>
+    </row>
+    <row r="405" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A405">
+        <v>148</v>
+      </c>
+      <c r="B405" s="5">
+        <v>41850</v>
+      </c>
+      <c r="C405" s="4">
+        <v>0.72916666666667596</v>
+      </c>
+    </row>
+    <row r="406" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A406">
+        <v>70</v>
+      </c>
+      <c r="B406" s="5">
+        <v>41850</v>
+      </c>
+      <c r="C406" s="4">
+        <v>0.75000000000000999</v>
+      </c>
+    </row>
+    <row r="407" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A407">
+        <v>49</v>
+      </c>
+      <c r="B407" s="5">
+        <v>41850</v>
+      </c>
+      <c r="C407" s="4">
+        <v>0.77083333333334403</v>
+      </c>
+    </row>
+    <row r="408" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A408">
+        <v>1</v>
+      </c>
+      <c r="B408" s="5">
+        <v>41851</v>
+      </c>
+      <c r="C408" s="4">
+        <v>0.29166666666666669</v>
+      </c>
+    </row>
+    <row r="409" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A409">
+        <v>3</v>
+      </c>
+      <c r="B409" s="5">
+        <v>41851</v>
+      </c>
+      <c r="C409" s="4">
+        <v>0.3125</v>
+      </c>
+    </row>
+    <row r="410" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A410">
+        <v>11</v>
+      </c>
+      <c r="B410" s="5">
+        <v>41851</v>
+      </c>
+      <c r="C410" s="4">
+        <v>0.33333333333333298</v>
+      </c>
+    </row>
+    <row r="411" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A411">
+        <v>34</v>
+      </c>
+      <c r="B411" s="5">
+        <v>41851</v>
+      </c>
+      <c r="C411" s="4">
+        <v>0.35416666666666702</v>
+      </c>
+    </row>
+    <row r="412" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A412">
+        <v>94</v>
+      </c>
+      <c r="B412" s="5">
+        <v>41851</v>
+      </c>
+      <c r="C412" s="4">
+        <v>0.375</v>
+      </c>
+    </row>
+    <row r="413" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A413">
+        <v>159</v>
+      </c>
+      <c r="B413" s="5">
+        <v>41851</v>
+      </c>
+      <c r="C413" s="4">
+        <v>0.39583333333333398</v>
+      </c>
+    </row>
+    <row r="414" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A414">
+        <v>184</v>
+      </c>
+      <c r="B414" s="5">
+        <v>41851</v>
+      </c>
+      <c r="C414" s="4">
+        <v>0.41666666666666702</v>
+      </c>
+    </row>
+    <row r="415" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A415">
+        <v>205</v>
+      </c>
+      <c r="B415" s="5">
+        <v>41851</v>
+      </c>
+      <c r="C415" s="4">
+        <v>0.4375</v>
+      </c>
+    </row>
+    <row r="416" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A416">
+        <v>214</v>
+      </c>
+      <c r="B416" s="5">
+        <v>41851</v>
+      </c>
+      <c r="C416" s="4">
+        <v>0.45833333333333398</v>
+      </c>
+    </row>
+    <row r="417" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A417">
+        <v>229</v>
+      </c>
+      <c r="B417" s="5">
+        <v>41851</v>
+      </c>
+      <c r="C417" s="4">
+        <v>0.47916666666666702</v>
+      </c>
+    </row>
+    <row r="418" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A418">
+        <v>237</v>
+      </c>
+      <c r="B418" s="5">
+        <v>41851</v>
+      </c>
+      <c r="C418" s="4">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="419" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A419">
+        <v>240</v>
+      </c>
+      <c r="B419" s="5">
+        <v>41851</v>
+      </c>
+      <c r="C419" s="4">
+        <v>0.52083333333333304</v>
+      </c>
+    </row>
+    <row r="420" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B420" s="5">
+        <v>41851</v>
+      </c>
+      <c r="C420" s="4">
+        <v>0.54166666666666596</v>
+      </c>
+    </row>
+    <row r="421" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B421" s="5">
+        <v>41851</v>
+      </c>
+      <c r="C421" s="4">
+        <v>0.562499999999999</v>
+      </c>
+    </row>
+    <row r="422" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B422" s="5">
+        <v>41851</v>
+      </c>
+      <c r="C422" s="4">
+        <v>0.58333333333333204</v>
+      </c>
+    </row>
+    <row r="423" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B423" s="5">
+        <v>41851</v>
+      </c>
+      <c r="C423" s="4">
+        <v>0.60416666666666496</v>
+      </c>
+    </row>
+    <row r="424" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B424" s="5">
+        <v>41851</v>
+      </c>
+      <c r="C424" s="4">
+        <v>0.624999999999998</v>
+      </c>
+    </row>
+    <row r="425" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B425" s="5">
+        <v>41851</v>
+      </c>
+      <c r="C425" s="4">
+        <v>0.64583333333333104</v>
+      </c>
+    </row>
+    <row r="426" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B426" s="5">
+        <v>41851</v>
+      </c>
+      <c r="C426" s="4">
+        <v>0.66666666666666397</v>
+      </c>
+    </row>
+    <row r="427" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B427" s="5">
+        <v>41851</v>
+      </c>
+      <c r="C427" s="4">
+        <v>0.687499999999997</v>
+      </c>
+    </row>
+    <row r="428" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B428" s="5">
+        <v>41851</v>
+      </c>
+      <c r="C428" s="4">
+        <v>0.70833333333333004</v>
+      </c>
+    </row>
+    <row r="429" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B429" s="5">
+        <v>41851</v>
+      </c>
+      <c r="C429" s="4">
+        <v>0.72916666666666297</v>
+      </c>
+    </row>
+    <row r="430" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B430" s="5">
+        <v>41851</v>
+      </c>
+      <c r="C430" s="4">
+        <v>0.749999999999997</v>
+      </c>
+    </row>
+    <row r="431" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B431" s="5">
+        <v>41851</v>
+      </c>
+      <c r="C431" s="4">
+        <v>0.77083333333333004</v>
+      </c>
+    </row>
+    <row r="432" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B432" s="5">
+        <v>41851</v>
+      </c>
+    </row>
+    <row r="433" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B433" s="5">
+        <v>41851</v>
+      </c>
+    </row>
+    <row r="434" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B434" s="5">
+        <v>41851</v>
+      </c>
+    </row>
+    <row r="435" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B435" s="5">
+        <v>41851</v>
+      </c>
+    </row>
+    <row r="436" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B436" s="5">
+        <v>41851</v>
+      </c>
+    </row>
+    <row r="437" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B437" s="5">
+        <v>41851</v>
+      </c>
+    </row>
+    <row r="438" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B438" s="5">
+        <v>41851</v>
+      </c>
+    </row>
+    <row r="439" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B439" s="5">
+        <v>41851</v>
+      </c>
+    </row>
+    <row r="440" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B440" s="5">
+        <v>41851</v>
+      </c>
+    </row>
+    <row r="441" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B441" s="5">
+        <v>41851</v>
+      </c>
+    </row>
+    <row r="442" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B442" s="5">
+        <v>41851</v>
+      </c>
+    </row>
+    <row r="443" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B443" s="5">
+        <v>41851</v>
+      </c>
+    </row>
+    <row r="444" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B444" s="5">
+        <v>41851</v>
+      </c>
+    </row>
+    <row r="445" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B445" s="5">
+        <v>41851</v>
+      </c>
+    </row>
+    <row r="446" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B446" s="5">
+        <v>41851</v>
+      </c>
+    </row>
+    <row r="447" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B447" s="5">
+        <v>41851</v>
+      </c>
+    </row>
+    <row r="448" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B448" s="5">
+        <v>41851</v>
+      </c>
+    </row>
+    <row r="449" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B449" s="5">
+        <v>41851</v>
+      </c>
+    </row>
+    <row r="452" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A452" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="403" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A403" t="s">
+    <row r="453" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A453" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="404" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A404" t="s">
+    <row r="454" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A454" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="405" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A405" t="s">
+    <row r="455" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A455" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="406" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A406" t="s">
+    <row r="456" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A456" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="408" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A408" t="s">
+    <row r="458" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A458" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="409" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A409" t="s">
+    <row r="459" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A459" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="410" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A410" t="s">
+    <row r="460" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A460" t="s">
         <v>1</v>
       </c>
     </row>

</xml_diff>